<commit_message>
Fixed excel script (pages situation)
</commit_message>
<xml_diff>
--- a/static/result/average_prices.xlsx
+++ b/static/result/average_prices.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1323.065436651953</v>
+        <v>1575.477723373003</v>
       </c>
       <c r="C2" t="n">
-        <v>1323.065436651953</v>
+        <v>1575.477723373003</v>
       </c>
       <c r="D2" t="n">
-        <v>1318.073873187994</v>
+        <v>1572.299293773217</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1243.46051101805</v>
+        <v>1600.019014252174</v>
       </c>
       <c r="C3" t="n">
-        <v>1243.46051101805</v>
+        <v>1600.019014252174</v>
       </c>
       <c r="D3" t="n">
-        <v>1236.34319051374</v>
+        <v>1597.763145621847</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1328.442742819084</v>
+        <v>1616.886424091637</v>
       </c>
       <c r="C4" t="n">
-        <v>1331.017664002765</v>
+        <v>1626.258828749242</v>
       </c>
       <c r="D4" t="n">
-        <v>1328.442742819084</v>
+        <v>1616.886424091637</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1389.568146707205</v>
+        <v>1734.312784874813</v>
       </c>
       <c r="C5" t="n">
-        <v>1398.155992508945</v>
+        <v>1748.71612779832</v>
       </c>
       <c r="D5" t="n">
-        <v>1389.568146707205</v>
+        <v>1734.312784874813</v>
       </c>
     </row>
     <row r="6">
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1444.167130496976</v>
+        <v>1782.202981048386</v>
       </c>
       <c r="C6" t="n">
-        <v>1448.94088646872</v>
+        <v>1790.543296175052</v>
       </c>
       <c r="D6" t="n">
-        <v>1444.167130496976</v>
+        <v>1782.202981048386</v>
       </c>
     </row>
     <row r="7">
@@ -542,10 +542,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1447.539105260941</v>
+        <v>1733.711422127711</v>
       </c>
       <c r="C7" t="n">
-        <v>1447.539105260941</v>
+        <v>1733.711422127711</v>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
@@ -556,10 +556,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1591.220132333171</v>
+        <v>1694.094743154283</v>
       </c>
       <c r="C8" t="n">
-        <v>1591.220132333171</v>
+        <v>1694.094743154283</v>
       </c>
       <c r="D8" t="inlineStr"/>
     </row>
@@ -570,13 +570,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1545.867619043562</v>
+        <v>1730.260844539496</v>
       </c>
       <c r="C9" t="n">
-        <v>1593.518390982004</v>
+        <v>1747.653453086408</v>
       </c>
       <c r="D9" t="n">
-        <v>1545.867619043562</v>
+        <v>1730.260844539496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>